<commit_message>
Add Ships and Water Requirements dashboards with charts and data loaders
</commit_message>
<xml_diff>
--- a/data/Greeceplots_uses.xlsx
+++ b/data/Greeceplots_uses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\FR1PEPF00001037\EXCELCNV\7068999d-201e-4ed9-b892-86b64803ef1d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\LN2PEPF0000C30F\EXCELCNV\f359cebe-dc5a-4981-9f85-b27450e8ab35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2071B821-4EB3-4CCE-802B-54D47568E413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C781E94-B36C-420B-B2F7-3B860C27F67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{C9D136AB-618D-4709-A6EB-9E1560B809B7}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{C2436BA9-935F-49C8-B9CF-C2E757A46CC0}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -905,7 +905,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6080EE15-08B5-4AB0-B10D-4B24618D90FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAF3D03-8667-4193-A1E1-D4187B80EF21}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>